<commit_message>
Powerplant energy production simulation
</commit_message>
<xml_diff>
--- a/regional_simulator/power_plants_2019.xlsx
+++ b/regional_simulator/power_plants_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\Git\Energy-Grid-Backend\regional_simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D76AF6-3B64-4D68-8B34-371C133007B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5059AFEB-B496-4786-A39D-A45AFA453C1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3984" yWindow="2520" windowWidth="17280" windowHeight="8964" xr2:uid="{B9ADFFCA-05C2-47E4-A404-671382D5D726}"/>
+    <workbookView xWindow="4332" yWindow="2868" windowWidth="17280" windowHeight="8964" xr2:uid="{B9ADFFCA-05C2-47E4-A404-671382D5D726}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>FUELTYPE</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Getijden</t>
+  </si>
+  <si>
+    <t>CURRENT_CAPACITY</t>
   </si>
 </sst>
 </file>
@@ -414,19 +417,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E79AC2D-A6A8-475B-8FEC-4019FAB7009E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -436,8 +440,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -447,8 +454,11 @@
       <c r="C2">
         <v>485000</v>
       </c>
+      <c r="D2">
+        <v>80</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -458,8 +468,11 @@
       <c r="C3">
         <v>435000</v>
       </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -469,8 +482,11 @@
       <c r="C4">
         <v>435000</v>
       </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -479,6 +495,9 @@
       </c>
       <c r="C5">
         <v>1200</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
power plant simulation refactor
</commit_message>
<xml_diff>
--- a/regional_simulator/power_plants_2019.xlsx
+++ b/regional_simulator/power_plants_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\Git\Energy-Grid-Backend\regional_simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5059AFEB-B496-4786-A39D-A45AFA453C1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356C2B18-F818-44E2-905F-62FA9A8DEAD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4332" yWindow="2868" windowWidth="17280" windowHeight="8964" xr2:uid="{B9ADFFCA-05C2-47E4-A404-671382D5D726}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>